<commit_message>
✨ Add TAS2 Form.
</commit_message>
<xml_diff>
--- a/LF/TAS/Benin/bj_lf_tas2_1_sites_202006.xlsx
+++ b/LF/TAS/Benin/bj_lf_tas2_1_sites_202006.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Benin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C661A6A5-F553-43D4-B0C2-045FABD8AD5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0064BE0F-3EEC-41DF-993B-C4FE393D6ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
   <si>
     <t>form_title</t>
   </si>
@@ -224,12 +224,6 @@
     <t>regex(.,'^[0-9]{2}$')</t>
   </si>
   <si>
-    <t>The code must be a two-digit number between 9 and 1000</t>
-  </si>
-  <si>
-    <t>Le code doit être un nombre à deux chiffres entre 9 et 1000</t>
-  </si>
-  <si>
     <t>Sélectionner l'unité d'évaluation (UE)</t>
   </si>
   <si>
@@ -303,6 +297,42 @@
   </si>
   <si>
     <t>eu_list = ${c_eu_name}</t>
+  </si>
+  <si>
+    <t>The code must be a two-digit number between 9 and 100</t>
+  </si>
+  <si>
+    <t>Le code doit être un nombre à deux chiffres entre 9 et 100</t>
+  </si>
+  <si>
+    <t>The number of presents must not exceed the total of pupils</t>
+  </si>
+  <si>
+    <t>The number of absents must not exceed the total of pupils</t>
+  </si>
+  <si>
+    <t>Le nombre d'absents  ne doit pas dépasser le total d'élèves</t>
+  </si>
+  <si>
+    <t>Le nombre des présents ne doit pas dépasser le total d'élèves</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>p_ending_survey_note</t>
+  </si>
+  <si>
+    <t>You just entered a value that will end the survey</t>
+  </si>
+  <si>
+    <t>Vous vener de saisir une valeur qui mettra fin à l'enquête</t>
+  </si>
+  <si>
+    <t>${c_consent} = 'No'</t>
+  </si>
+  <si>
+    <t>${c_consent} = 'Yes'</t>
   </si>
 </sst>
 </file>
@@ -434,7 +464,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -521,6 +551,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -810,13 +843,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -913,10 +946,10 @@
         <v>63</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
@@ -932,14 +965,14 @@
         <v>45</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="14"/>
@@ -957,13 +990,13 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
@@ -982,7 +1015,7 @@
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
       <c r="P4" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -990,14 +1023,14 @@
         <v>46</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="9"/>
@@ -1018,14 +1051,14 @@
         <v>46</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="9"/>
@@ -1041,86 +1074,92 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="14"/>
       <c r="M8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:16" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="L9" s="8"/>
       <c r="M9" s="9" t="s">
         <v>57</v>
@@ -1129,26 +1168,34 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>27</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="L10" s="8"/>
       <c r="M10" s="9" t="s">
         <v>57</v>
@@ -1180,7 +1227,9 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
         <v>57</v>
@@ -1189,44 +1238,40 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>31</v>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="F12" s="21"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="K12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="F13" s="21"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1241,10 +1286,10 @@
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>34</v>
@@ -1262,6 +1307,30 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1308,13 +1377,13 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="26"/>
     </row>
@@ -1323,13 +1392,13 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="26"/>
     </row>
@@ -1338,13 +1407,13 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -1353,19 +1422,19 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>101</v>
@@ -1377,12 +1446,12 @@
         <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>102</v>
@@ -1394,12 +1463,12 @@
         <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>103</v>
@@ -1411,12 +1480,12 @@
         <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9">
         <v>104</v>
@@ -1428,7 +1497,7 @@
         <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1473,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1509,7 +1578,7 @@
         <v>20200601</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>